<commit_message>
Updated the files with new lines of code and visualisations
</commit_message>
<xml_diff>
--- a/Exp sem.xlsx
+++ b/Exp sem.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="270">
   <si>
     <t xml:space="preserve">Bibliographical reference</t>
   </si>
@@ -695,9 +695,6 @@
   </si>
   <si>
     <t xml:space="preserve">3 - symbols</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
   </si>
   <si>
     <t xml:space="preserve">online</t>
@@ -1408,8 +1405,8 @@
   </sheetPr>
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R34" activeCellId="0" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2243,6 +2240,12 @@
       <c r="O12" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="P12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="S12" s="4" t="n">
         <v>1</v>
       </c>
@@ -3208,7 +3211,9 @@
       <c r="M26" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="N26" s="4"/>
+      <c r="N26" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="O26" s="4" t="n">
         <v>1</v>
       </c>
@@ -3700,37 +3705,37 @@
       <c r="O33" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="P33" s="7" t="s">
+      <c r="P33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="Q33" s="7" t="s">
+      <c r="R33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T33" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U33" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="V33" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="R33" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="S33" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="T33" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="U33" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="V33" s="10" t="s">
+      <c r="W33" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="W33" s="4" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" s="18" t="s">
         <v>168</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>169</v>
       </c>
       <c r="C34" s="10" t="n">
         <v>2016</v>
@@ -3792,15 +3797,15 @@
         <v>1</v>
       </c>
       <c r="W34" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>2009</v>
@@ -3823,22 +3828,22 @@
         <v>2</v>
       </c>
       <c r="J35" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="K35" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M35" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N35" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="K35" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L35" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="M35" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="N35" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O35" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="P35" s="7" t="n">
         <v>3</v>
@@ -3867,10 +3872,10 @@
     </row>
     <row r="36" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>175</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>176</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>2018</v>
@@ -3893,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K36" s="4" t="n">
         <v>2</v>
@@ -3932,15 +3937,15 @@
         <v>1</v>
       </c>
       <c r="W36" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="225" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>179</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>180</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>2009</v>
@@ -3963,7 +3968,7 @@
         <v>2</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K37" s="4" t="n">
         <v>1</v>
@@ -4007,10 +4012,10 @@
     </row>
     <row r="38" customFormat="false" ht="216" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" s="20" t="s">
         <v>182</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>183</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>2014</v>
@@ -4033,7 +4038,7 @@
         <v>1</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K38" s="4" t="n">
         <v>2</v>
@@ -4072,15 +4077,15 @@
         <v>1</v>
       </c>
       <c r="W38" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>187</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>2018</v>
@@ -4112,19 +4117,19 @@
         <v>1</v>
       </c>
       <c r="M39" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="N39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O39" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="N39" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="O39" s="4" t="s">
-        <v>189</v>
-      </c>
       <c r="P39" s="7" t="n">
         <v>3</v>
       </c>
       <c r="Q39" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R39" s="7" t="n">
         <v>719</v>
@@ -4133,24 +4138,24 @@
         <v>1</v>
       </c>
       <c r="T39" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="U39" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="V39" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="W39" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="U39" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="V39" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="W39" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>192</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>193</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>2015</v>
@@ -4173,7 +4178,7 @@
         <v>1</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K40" s="4" t="n">
         <v>2</v>
@@ -4212,15 +4217,15 @@
         <v>1</v>
       </c>
       <c r="W40" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="225" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>196</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>197</v>
       </c>
       <c r="C41" s="15" t="n">
         <v>2019</v>
@@ -4243,10 +4248,10 @@
         <v>1</v>
       </c>
       <c r="J41" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="K41" s="15" t="s">
         <v>198</v>
-      </c>
-      <c r="K41" s="15" t="s">
-        <v>199</v>
       </c>
       <c r="L41" s="15" t="n">
         <v>1</v>
@@ -4282,15 +4287,15 @@
         <v>1</v>
       </c>
       <c r="W41" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>201</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>202</v>
       </c>
       <c r="C42" s="15" t="n">
         <v>2019</v>
@@ -4313,7 +4318,7 @@
         <v>1</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K42" s="15" t="n">
         <v>2</v>
@@ -4350,15 +4355,15 @@
         <v>1</v>
       </c>
       <c r="W42" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B43" s="22" t="s">
         <v>204</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>205</v>
       </c>
       <c r="C43" s="15" t="n">
         <v>2020</v>
@@ -4381,7 +4386,7 @@
         <v>1</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K43" s="15" t="n">
         <v>2</v>
@@ -4420,15 +4425,15 @@
         <v>1</v>
       </c>
       <c r="W43" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>206</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>207</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>2020</v>
@@ -4490,15 +4495,15 @@
         <v>1</v>
       </c>
       <c r="W44" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>209</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>210</v>
       </c>
       <c r="C45" s="4" t="n">
         <v>2020</v>
@@ -4521,7 +4526,7 @@
         <v>1</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K45" s="4" t="n">
         <v>3</v>
@@ -4560,15 +4565,15 @@
         <v>1</v>
       </c>
       <c r="W45" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>214</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>2012</v>
@@ -4591,13 +4596,13 @@
         <v>1</v>
       </c>
       <c r="J46" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="K46" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L46" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="K46" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="L46" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="M46" s="4" t="n">
         <v>3</v>
@@ -4630,15 +4635,15 @@
         <v>1</v>
       </c>
       <c r="W46" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="225" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="C47" s="4" t="n">
         <v>2015</v>
@@ -4661,7 +4666,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K47" s="4" t="n">
         <v>2</v>
@@ -4700,15 +4705,15 @@
         <v>1</v>
       </c>
       <c r="W47" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B48" s="11" t="s">
         <v>220</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>221</v>
       </c>
       <c r="C48" s="4" t="n">
         <v>2018</v>
@@ -4725,28 +4730,28 @@
         <v>2</v>
       </c>
       <c r="H48" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="J48" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="I48" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="J48" s="6" t="s">
+      <c r="K48" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="K48" s="10" t="s">
+      <c r="L48" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="L48" s="4" t="s">
+      <c r="M48" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="M48" s="4" t="s">
-        <v>226</v>
-      </c>
       <c r="N48" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O48" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P48" s="7" t="n">
         <v>3</v>
@@ -4758,16 +4763,16 @@
         <v>12</v>
       </c>
       <c r="S48" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T48" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U48" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V48" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="W48" s="4" t="n">
         <v>0</v>
@@ -4775,10 +4780,10 @@
     </row>
     <row r="49" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>227</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>228</v>
       </c>
       <c r="C49" s="4" t="n">
         <v>2009</v>
@@ -4801,7 +4806,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K49" s="4" t="n">
         <v>1</v>
@@ -4840,15 +4845,15 @@
         <v>1</v>
       </c>
       <c r="W49" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="310.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>232</v>
       </c>
       <c r="C50" s="4" t="n">
         <v>2007</v>
@@ -4871,7 +4876,7 @@
         <v>1</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K50" s="4" t="n">
         <v>1</v>
@@ -4915,10 +4920,10 @@
     </row>
     <row r="51" customFormat="false" ht="377.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B51" s="9" t="s">
         <v>234</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>235</v>
       </c>
       <c r="C51" s="4" t="n">
         <v>2019</v>
@@ -4935,28 +4940,28 @@
         <v>3.33333333333333</v>
       </c>
       <c r="H51" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="I51" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="J51" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="J51" s="6" t="s">
+      <c r="K51" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L51" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="K51" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="L51" s="4" t="s">
+      <c r="M51" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="M51" s="4" t="s">
-        <v>240</v>
-      </c>
       <c r="N51" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P51" s="7" t="n">
         <v>2</v>
@@ -4968,27 +4973,27 @@
         <v>43</v>
       </c>
       <c r="S51" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T51" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="U51" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="V51" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="W51" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="225" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B52" s="9" t="s">
         <v>242</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>243</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>2019</v>
@@ -5050,15 +5055,15 @@
         <v>1</v>
       </c>
       <c r="W52" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B53" s="11" t="s">
         <v>245</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>246</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>2014</v>
@@ -5081,22 +5086,22 @@
         <v>2</v>
       </c>
       <c r="J53" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="K53" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L53" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M53" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N53" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O53" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="K53" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L53" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="M53" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="N53" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O53" s="4" t="s">
-        <v>248</v>
       </c>
       <c r="P53" s="7" t="n">
         <v>3</v>
@@ -5125,10 +5130,10 @@
     </row>
     <row r="54" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B54" s="9" t="s">
         <v>249</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>250</v>
       </c>
       <c r="C54" s="4" t="n">
         <v>2013</v>
@@ -5151,7 +5156,7 @@
         <v>2</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K54" s="4" t="n">
         <v>1</v>
@@ -5195,10 +5200,10 @@
     </row>
     <row r="55" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>252</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>253</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>2010</v>
@@ -5221,7 +5226,7 @@
         <v>1</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K55" s="4" t="n">
         <v>2</v>
@@ -5260,15 +5265,15 @@
         <v>1</v>
       </c>
       <c r="W55" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B56" s="11" t="s">
         <v>256</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>257</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>2012</v>
@@ -5291,7 +5296,7 @@
         <v>2</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K56" s="4" t="n">
         <v>1</v>
@@ -5335,10 +5340,10 @@
     </row>
     <row r="57" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B57" s="11" t="s">
         <v>259</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>260</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>2011</v>
@@ -5361,7 +5366,7 @@
         <v>2</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K57" s="4" t="n">
         <v>1</v>
@@ -5405,10 +5410,10 @@
     </row>
     <row r="58" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>261</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>262</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>2017</v>
@@ -5431,22 +5436,22 @@
         <v>1</v>
       </c>
       <c r="J58" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="K58" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L58" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M58" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N58" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O58" s="4" t="s">
         <v>263</v>
-      </c>
-      <c r="K58" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="L58" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M58" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N58" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O58" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="P58" s="7" t="n">
         <v>2</v>
@@ -5470,15 +5475,15 @@
         <v>2</v>
       </c>
       <c r="W58" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="297" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>266</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>267</v>
       </c>
       <c r="C59" s="4" t="n">
         <v>2021</v>
@@ -5501,22 +5506,22 @@
         <v>1</v>
       </c>
       <c r="J59" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="K59" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L59" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M59" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N59" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O59" s="10" t="s">
         <v>268</v>
-      </c>
-      <c r="K59" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="L59" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M59" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N59" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O59" s="10" t="s">
-        <v>269</v>
       </c>
       <c r="P59" s="7" t="n">
         <v>3</v>
@@ -5540,7 +5545,7 @@
         <v>2</v>
       </c>
       <c r="W59" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>